<commit_message>
Practice Excel, using Solver
</commit_message>
<xml_diff>
--- a/Excel/AirlineRM_Connecting_Complete.xlsx
+++ b/Excel/AirlineRM_Connecting_Complete.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14020" windowHeight="15160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="15165" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,11 @@
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$15:$B$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$E$5:$E$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$E$5:$E$10</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -24,14 +26,17 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$12</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$D$15:$D$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$D$5:$D$10</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$D$15</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$D$16</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$D$5:$D$10</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -41,9 +46,9 @@
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -268,6 +273,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -596,15 +606,15 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -615,7 +625,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -624,7 +634,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="16" thickBot="1">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -637,7 +647,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="16" thickBot="1">
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
@@ -652,7 +662,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="16" thickBot="1">
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -663,15 +673,15 @@
         <v>428</v>
       </c>
       <c r="D5" s="4">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E5" s="5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16" thickBot="1">
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -688,7 +698,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="16" thickBot="1">
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -707,7 +717,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="16" thickBot="1">
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -719,12 +729,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1">
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -743,7 +753,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1">
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -755,12 +765,12 @@
         <v>110</v>
       </c>
       <c r="E10" s="5">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="16" thickBot="1">
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -769,21 +779,28 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="16" thickBot="1">
+    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="7">
         <f>SUMPRODUCT(C5:C10,E5:E10)</f>
+        <v>120654</v>
+      </c>
+      <c r="C12" s="1">
         <v>120514</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1">
+        <v>120654</v>
+      </c>
+      <c r="E12" s="1">
+        <f>C12-D12</f>
+        <v>-140</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -792,7 +809,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="16" thickBot="1">
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -809,7 +826,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="16" thickBot="1">
+    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -827,7 +844,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="16" thickBot="1">
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -845,7 +862,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1">
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -862,7 +879,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="16" thickBot="1">
+    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>